<commit_message>
Forget Password and Change Password
</commit_message>
<xml_diff>
--- a/website/csv_files/Books_Download.xlsx
+++ b/website/csv_files/Books_Download.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -480,29 +480,29 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C2" t="n">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>edited dskjvbds</t>
+          <t>sdvkjdsnvkj edited</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>kjsdvkjs edited</t>
+          <t>fsdklnvdsklvn</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>jkvsdkj</t>
+          <t>knsdkjvndsk</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>bdskjvk</t>
+          <t>nvkjwnvkjsd</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -512,7 +512,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>dskjvdskj</t>
+          <t>knfdklvnsdl</t>
         </is>
       </c>
     </row>
@@ -521,29 +521,29 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C3" t="n">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>sdkjvnsdk</t>
+          <t>sdvkjdsnvkjds</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>dvskjvhsdk</t>
+          <t>nvsbkdjbvsnk</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>skjdvs</t>
+          <t>sdvnkjvnsdk</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>jdksdhvn</t>
+          <t>kjsdbvkdsj</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -553,48 +553,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>vdsnkjkcjf</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>7</v>
-      </c>
-      <c r="C4" t="n">
-        <v>8</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>s,mvsd bhvj</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>dvsh jk</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>mknsd hj</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>kmjsdh</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>1975</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>ds ha</t>
+          <t>nvfksjdnvs</t>
         </is>
       </c>
     </row>

</xml_diff>